<commit_message>
Componsant LWC TableauLivraison cree
</commit_message>
<xml_diff>
--- a/data/Prix.xlsx
+++ b/data/Prix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\CODE SALES FORCES\PROJET 7\PROJET7\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEED28EC-715A-4D7E-8210-A7D770A5B48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2A8E0A-BB27-4DD5-A5B3-4DF8F88C4A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B9CE6759-FA50-4105-AB14-5C5211C54719}"/>
   </bookViews>
@@ -21,7 +21,20 @@
     <definedName name="DonnéesExternes_1" localSheetId="0" hidden="1">'Prix (2)'!$A$1:$D$47</definedName>
     <definedName name="DonnéesExternes_1" localSheetId="1" hidden="1">TRANSPORTEUR!$A$1:$E$16</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -652,9 +665,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -756,13 +768,19 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DE9DDC8F-04A9-48C9-9604-4F938B9C4512}" name="Prix" displayName="Prix" ref="A1:E47" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E47" xr:uid="{DE9DDC8F-04A9-48C9-9604-4F938B9C4512}"/>
+  <autoFilter ref="A1:E47" xr:uid="{DE9DDC8F-04A9-48C9-9604-4F938B9C4512}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Belgique"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{53811DFC-F3AA-4355-82DA-08E5602C7F29}" uniqueName="1" name="Transporteur ID" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{91E245DF-2E05-4BE3-8303-9D8E48A2B2A9}" uniqueName="2" name="Pays" queryTableFieldId="2" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{0B5ED397-0819-4102-A800-A75C28360377}" uniqueName="3" name="Tarif" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{92B1624F-F9B6-4CE3-A67B-F46D6B968524}" uniqueName="4" name="Délai de Livraison (jours)" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{352004F3-9B15-44D9-B95B-BE1356FA396A}" uniqueName="5" name="IDTRANSPORTEUR" queryTableFieldId="5" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{352004F3-9B15-44D9-B95B-BE1356FA396A}" uniqueName="5" name="IDTRANSPORTEUR" queryTableFieldId="5" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(A2,TRANSPORTEUR!$A$1:$B$16,2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -775,10 +793,10 @@
   <autoFilter ref="A1:E16" xr:uid="{5F521D3E-8AE8-4633-B8D9-02D47FC92A4F}"/>
   <tableColumns count="5">
     <tableColumn id="5" xr3:uid="{10A6C880-B36C-4D64-8944-122B50427DCC}" uniqueName="5" name="TransporteurId" queryTableFieldId="5"/>
-    <tableColumn id="1" xr3:uid="{3E6E7847-6374-4B45-A70A-EEA9DC6E3037}" uniqueName="1" name="Record ID" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3E6E7847-6374-4B45-A70A-EEA9DC6E3037}" uniqueName="1" name="Record ID" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{AEC1CE55-0363-4A50-9233-3351722E8562}" uniqueName="2" name="PourParticulier" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{69E2CEDA-4CC2-4D42-A8B0-95F9A06FB1AF}" uniqueName="3" name="PourProfessionnel" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{821BE241-AD21-41DD-98EC-F763BE133E2A}" uniqueName="4" name="Transporteur Name" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{821BE241-AD21-41DD-98EC-F763BE133E2A}" uniqueName="4" name="Transporteur Name" queryTableFieldId="4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1103,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480B46E0-4BFD-468D-AA9B-A85400F72768}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1133,11 +1151,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2">
@@ -1155,7 +1173,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3">
@@ -1169,11 +1187,11 @@
         <v>a00Qy00000it6OPIAY</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4">
@@ -1187,11 +1205,11 @@
         <v>a00Qy00000it6OPIAY</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5">
@@ -1205,11 +1223,11 @@
         <v>a00Qy00000it6OPIAY</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
@@ -1227,7 +1245,7 @@
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7">
@@ -1241,11 +1259,11 @@
         <v>a00Qy00000it6OQIAY</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8">
@@ -1259,11 +1277,11 @@
         <v>a00Qy00000it6OQIAY</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9">
@@ -1277,11 +1295,11 @@
         <v>a00Qy00000it6OQIAY</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10">
@@ -1299,7 +1317,7 @@
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11">
@@ -1313,11 +1331,11 @@
         <v>a00Qy00000it6ORIAY</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12">
@@ -1335,7 +1353,7 @@
       <c r="A13">
         <v>4</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13">
@@ -1349,11 +1367,11 @@
         <v>a00Qy00000it6OSIAY</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14">
@@ -1367,11 +1385,11 @@
         <v>a00Qy00000it6OSIAY</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15">
@@ -1385,11 +1403,11 @@
         <v>a00Qy00000it6OSIAY</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>4</v>
       </c>
       <c r="C16">
@@ -1407,7 +1425,7 @@
       <c r="A17">
         <v>5</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17">
@@ -1421,11 +1439,11 @@
         <v>a00Qy00000it6OTIAY</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18">
@@ -1439,11 +1457,11 @@
         <v>a00Qy00000it6OTIAY</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19">
@@ -1457,11 +1475,11 @@
         <v>a00Qy00000it6OTIAY</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>4</v>
       </c>
       <c r="C20">
@@ -1475,11 +1493,11 @@
         <v>a00Qy00000it6OUIAY</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21">
@@ -1493,11 +1511,11 @@
         <v>a00Qy00000it6OUIAY</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>4</v>
       </c>
       <c r="C22">
@@ -1515,7 +1533,7 @@
       <c r="A23">
         <v>7</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23">
@@ -1529,11 +1547,11 @@
         <v>a00Qy00000it6OVIAY</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>8</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>6</v>
       </c>
       <c r="C24">
@@ -1547,11 +1565,11 @@
         <v>a00Qy00000it6OWIAY</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>8</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>7</v>
       </c>
       <c r="C25">
@@ -1565,11 +1583,11 @@
         <v>a00Qy00000it6OWIAY</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>4</v>
       </c>
       <c r="C26">
@@ -1587,7 +1605,7 @@
       <c r="A27">
         <v>9</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>5</v>
       </c>
       <c r="C27">
@@ -1601,11 +1619,11 @@
         <v>a00Qy00000it6OXIAY</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>4</v>
       </c>
       <c r="C28">
@@ -1619,11 +1637,11 @@
         <v>a00Qy00000it6OYIAY</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>6</v>
       </c>
       <c r="C29">
@@ -1637,11 +1655,11 @@
         <v>a00Qy00000it6OYIAY</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="C30">
@@ -1655,11 +1673,11 @@
         <v>a00Qy00000it6OYIAY</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>11</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>4</v>
       </c>
       <c r="C31">
@@ -1677,7 +1695,7 @@
       <c r="A32">
         <v>11</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>5</v>
       </c>
       <c r="C32">
@@ -1691,11 +1709,11 @@
         <v>a00Qy00000it6OZIAY</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>11</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>6</v>
       </c>
       <c r="C33">
@@ -1709,11 +1727,11 @@
         <v>a00Qy00000it6OZIAY</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>11</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>7</v>
       </c>
       <c r="C34">
@@ -1727,11 +1745,11 @@
         <v>a00Qy00000it6OZIAY</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>12</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>4</v>
       </c>
       <c r="C35">
@@ -1749,7 +1767,7 @@
       <c r="A36">
         <v>12</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>5</v>
       </c>
       <c r="C36">
@@ -1763,11 +1781,11 @@
         <v>a00Qy00000it6OaIAI</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>12</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>7</v>
       </c>
       <c r="C37">
@@ -1781,11 +1799,11 @@
         <v>a00Qy00000it6OaIAI</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>13</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>4</v>
       </c>
       <c r="C38">
@@ -1803,7 +1821,7 @@
       <c r="A39">
         <v>13</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>5</v>
       </c>
       <c r="C39">
@@ -1817,11 +1835,11 @@
         <v>a00Qy00000it6ObIAI</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>13</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>6</v>
       </c>
       <c r="C40">
@@ -1835,11 +1853,11 @@
         <v>a00Qy00000it6ObIAI</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>13</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>7</v>
       </c>
       <c r="C41">
@@ -1853,11 +1871,11 @@
         <v>a00Qy00000it6ObIAI</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>14</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>4</v>
       </c>
       <c r="C42">
@@ -1875,7 +1893,7 @@
       <c r="A43">
         <v>14</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>5</v>
       </c>
       <c r="C43">
@@ -1889,11 +1907,11 @@
         <v>a00Qy00000it6OcIAI</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>14</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>6</v>
       </c>
       <c r="C44">
@@ -1907,11 +1925,11 @@
         <v>a00Qy00000it6OcIAI</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>14</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>7</v>
       </c>
       <c r="C45">
@@ -1925,11 +1943,11 @@
         <v>a00Qy00000it6OcIAI</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>15</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>4</v>
       </c>
       <c r="C46">
@@ -1947,7 +1965,7 @@
       <c r="A47">
         <v>15</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>5</v>
       </c>
       <c r="C47">
@@ -2007,7 +2025,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="b">
@@ -2016,7 +2034,7 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2024,7 +2042,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="b">
@@ -2033,7 +2051,7 @@
       <c r="D3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2041,7 +2059,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>17</v>
       </c>
       <c r="C4" t="b">
@@ -2050,7 +2068,7 @@
       <c r="D4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2058,7 +2076,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" t="b">
@@ -2067,7 +2085,7 @@
       <c r="D5" t="b">
         <v>1</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2075,7 +2093,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="b">
@@ -2084,7 +2102,7 @@
       <c r="D6" t="b">
         <v>1</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2092,7 +2110,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="C7" t="b">
@@ -2101,7 +2119,7 @@
       <c r="D7" t="b">
         <v>0</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2109,7 +2127,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="C8" t="b">
@@ -2118,7 +2136,7 @@
       <c r="D8" t="b">
         <v>0</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2126,7 +2144,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="C9" t="b">
@@ -2135,7 +2153,7 @@
       <c r="D9" t="b">
         <v>1</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2143,7 +2161,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
       <c r="C10" t="b">
@@ -2152,7 +2170,7 @@
       <c r="D10" t="b">
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2160,7 +2178,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>31</v>
       </c>
       <c r="C11" t="b">
@@ -2169,7 +2187,7 @@
       <c r="D11" t="b">
         <v>1</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2177,7 +2195,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>33</v>
       </c>
       <c r="C12" t="b">
@@ -2186,7 +2204,7 @@
       <c r="D12" t="b">
         <v>1</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2194,7 +2212,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>35</v>
       </c>
       <c r="C13" t="b">
@@ -2203,7 +2221,7 @@
       <c r="D13" t="b">
         <v>0</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2211,7 +2229,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>37</v>
       </c>
       <c r="C14" t="b">
@@ -2220,7 +2238,7 @@
       <c r="D14" t="b">
         <v>1</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2228,7 +2246,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>39</v>
       </c>
       <c r="C15" t="b">
@@ -2237,7 +2255,7 @@
       <c r="D15" t="b">
         <v>1</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2245,7 +2263,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>41</v>
       </c>
       <c r="C16" t="b">
@@ -2254,7 +2272,7 @@
       <c r="D16" t="b">
         <v>0</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>